<commit_message>
Added draft events operation
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-subscription-notification.xlsx
+++ b/docs/StructureDefinition-backport-subscription-notification.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$83</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2811" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="251">
   <si>
     <t>Path</t>
   </si>
@@ -488,6 +488,50 @@
   </si>
   <si>
     <t>Bundle.entry.extension</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>focusResource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/uv/subscriptions-backport/StructureDefinition/subscription-notification-focus-resource}
+</t>
+  </si>
+  <si>
+    <t>Subscription Notification Focus Resource</t>
+  </si>
+  <si>
+    <t>Tagging for Bundle entries to indicate a resource is the focus of a specific notification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children unless an empty Parameters resource {hasValue() or (children().count() &gt; id.count()) or $this is Parameters}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>includedResource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/uv/subscriptions-backport/StructureDefinition/subscription-notification-included-resource}
+</t>
+  </si>
+  <si>
+    <t>Subscription Notification Included Resource</t>
+  </si>
+  <si>
+    <t>Tagging for Bundle entries to indicate a resource is included because of a specific notification.</t>
   </si>
   <si>
     <t>Bundle.entry.modifierExtension</t>
@@ -918,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM81"/>
+  <dimension ref="A1:AM83"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2968,7 +3012,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -2990,14 +3034,12 @@
         <v>120</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>40</v>
@@ -3034,16 +3076,14 @@
         <v>40</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB19" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="AB19" s="2"/>
       <c r="AC19" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD19" t="s" s="2">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="AE19" t="s" s="2">
         <v>124</v>
@@ -3064,7 +3104,7 @@
         <v>40</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>40</v>
@@ -3075,11 +3115,13 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="C20" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3092,26 +3134,22 @@
         <v>40</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>40</v>
       </c>
@@ -3159,7 +3197,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3168,16 +3206,16 @@
         <v>42</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>40</v>
@@ -3188,9 +3226,11 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="C21" t="s" s="2">
         <v>40</v>
       </c>
@@ -3208,16 +3248,16 @@
         <v>40</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3268,7 +3308,7 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
@@ -3277,10 +3317,10 @@
         <v>42</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>40</v>
@@ -3297,41 +3337,43 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>40</v>
       </c>
@@ -3379,25 +3421,25 @@
         <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>40</v>
@@ -3408,7 +3450,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3419,7 +3461,7 @@
         <v>41</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>40</v>
@@ -3431,13 +3473,13 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3488,19 +3530,19 @@
         <v>40</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>40</v>
@@ -3517,7 +3559,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3540,15 +3582,17 @@
         <v>51</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="M24" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>168</v>
+      </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -3597,7 +3641,7 @@
         <v>40</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -3606,10 +3650,10 @@
         <v>50</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>163</v>
+        <v>40</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>40</v>
@@ -3626,7 +3670,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3646,16 +3690,16 @@
         <v>40</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3706,7 +3750,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -3724,7 +3768,7 @@
         <v>40</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>40</v>
@@ -3735,18 +3779,18 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>40</v>
@@ -3755,20 +3799,18 @@
         <v>40</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>40</v>
@@ -3817,25 +3859,25 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>40</v>
@@ -3846,43 +3888,39 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>40</v>
       </c>
@@ -3930,25 +3968,25 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
@@ -3959,18 +3997,18 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>40</v>
@@ -3979,19 +4017,19 @@
         <v>40</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4017,13 +4055,13 @@
         <v>40</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>171</v>
+        <v>40</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>40</v>
@@ -4041,25 +4079,25 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>40</v>
@@ -4070,41 +4108,43 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>40</v>
       </c>
@@ -4152,25 +4192,25 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>40</v>
@@ -4181,7 +4221,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4204,15 +4244,17 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="M30" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>183</v>
+      </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>40</v>
@@ -4237,13 +4279,13 @@
         <v>40</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>40</v>
@@ -4261,7 +4303,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4270,10 +4312,10 @@
         <v>50</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>40</v>
@@ -4290,7 +4332,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4310,18 +4352,20 @@
         <v>40</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>189</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>40</v>
@@ -4370,7 +4414,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -4382,13 +4426,13 @@
         <v>40</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>40</v>
@@ -4399,18 +4443,18 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>40</v>
@@ -4419,20 +4463,18 @@
         <v>40</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>40</v>
@@ -4481,25 +4523,25 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>40</v>
@@ -4510,43 +4552,39 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>40</v>
       </c>
@@ -4594,25 +4632,25 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>40</v>
@@ -4623,18 +4661,18 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>40</v>
@@ -4643,18 +4681,20 @@
         <v>40</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>186</v>
+        <v>121</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>40</v>
@@ -4679,13 +4719,13 @@
         <v>40</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>40</v>
@@ -4703,25 +4743,25 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>40</v>
@@ -4732,41 +4772,43 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I35" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>191</v>
+        <v>128</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>40</v>
       </c>
@@ -4814,25 +4856,25 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>40</v>
@@ -4843,7 +4885,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4851,7 +4893,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>50</v>
@@ -4866,13 +4908,13 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -4899,13 +4941,13 @@
         <v>40</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>40</v>
@@ -4923,10 +4965,10 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>50</v>
@@ -4952,7 +4994,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -4960,7 +5002,7 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F37" t="s" s="2">
         <v>50</v>
@@ -4975,15 +5017,17 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>205</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>206</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>40</v>
@@ -5032,10 +5076,10 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>50</v>
@@ -5061,7 +5105,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5087,10 +5131,10 @@
         <v>133</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5141,7 +5185,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5170,7 +5214,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5193,13 +5237,13 @@
         <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5250,7 +5294,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5279,7 +5323,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5302,13 +5346,13 @@
         <v>51</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5359,7 +5403,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5368,10 +5412,10 @@
         <v>50</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>40</v>
@@ -5388,7 +5432,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5408,16 +5452,16 @@
         <v>40</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5468,7 +5512,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>116</v>
+        <v>215</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5480,13 +5524,13 @@
         <v>40</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>40</v>
@@ -5497,18 +5541,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>40</v>
@@ -5517,20 +5561,18 @@
         <v>40</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>40</v>
@@ -5579,25 +5621,25 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>124</v>
+        <v>218</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>40</v>
+        <v>221</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>40</v>
@@ -5608,43 +5650,39 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>40</v>
       </c>
@@ -5692,25 +5730,25 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>40</v>
@@ -5721,18 +5759,18 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>40</v>
@@ -5741,18 +5779,20 @@
         <v>40</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="M44" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>40</v>
@@ -5801,25 +5841,25 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>212</v>
+        <v>124</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>40</v>
@@ -5830,39 +5870,43 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I45" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>40</v>
       </c>
@@ -5910,25 +5954,25 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>215</v>
+        <v>131</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>40</v>
@@ -5939,7 +5983,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -5947,7 +5991,7 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s" s="2">
         <v>50</v>
@@ -5965,14 +6009,12 @@
         <v>133</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>221</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>40</v>
@@ -6021,10 +6063,10 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>50</v>
@@ -6050,7 +6092,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6073,17 +6115,15 @@
         <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>40</v>
@@ -6132,7 +6172,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6161,7 +6201,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6184,16 +6224,16 @@
         <v>51</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6243,7 +6283,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6255,7 +6295,7 @@
         <v>40</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>40</v>
@@ -6270,25 +6310,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>230</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F49" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>40</v>
@@ -6297,15 +6335,17 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>140</v>
+        <v>236</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="M49" s="2"/>
+        <v>237</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>238</v>
+      </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>40</v>
@@ -6354,19 +6394,19 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>139</v>
+        <v>235</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>145</v>
+        <v>62</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>40</v>
@@ -6383,7 +6423,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>146</v>
+        <v>239</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6403,18 +6443,20 @@
         <v>40</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>114</v>
+        <v>240</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M50" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>40</v>
@@ -6463,7 +6505,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>116</v>
+        <v>239</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -6481,7 +6523,7 @@
         <v>40</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
@@ -6490,42 +6532,42 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="B51" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>243</v>
+      </c>
       <c r="C51" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>40</v>
@@ -6574,7 +6616,7 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -6586,13 +6628,13 @@
         <v>40</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -6603,43 +6645,39 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>40</v>
       </c>
@@ -6687,25 +6725,25 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>40</v>
@@ -6716,11 +6754,11 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -6736,18 +6774,20 @@
         <v>40</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M53" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>40</v>
@@ -6796,7 +6836,7 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -6808,13 +6848,13 @@
         <v>40</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>40</v>
@@ -6825,41 +6865,43 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H54" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I54" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="N54" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
       </c>
@@ -6907,25 +6949,25 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>40</v>
@@ -6934,9 +6976,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -6944,13 +6986,13 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>40</v>
@@ -6959,13 +7001,13 @@
         <v>51</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>231</v>
+        <v>40</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7016,19 +7058,19 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>40</v>
@@ -7045,7 +7087,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7068,15 +7110,17 @@
         <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="M56" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>168</v>
+      </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>40</v>
@@ -7125,7 +7169,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7134,10 +7178,10 @@
         <v>50</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>163</v>
+        <v>40</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>40</v>
@@ -7152,9 +7196,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7162,28 +7206,28 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7234,7 +7278,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7252,7 +7296,7 @@
         <v>40</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
@@ -7263,18 +7307,18 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>40</v>
@@ -7283,20 +7327,18 @@
         <v>40</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>40</v>
@@ -7345,25 +7387,25 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
@@ -7374,43 +7416,39 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H59" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>40</v>
       </c>
@@ -7458,25 +7496,25 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
@@ -7487,18 +7525,18 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>40</v>
@@ -7507,19 +7545,19 @@
         <v>40</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -7545,13 +7583,13 @@
         <v>40</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>171</v>
+        <v>40</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>172</v>
+        <v>40</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>40</v>
@@ -7569,25 +7607,25 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
@@ -7598,41 +7636,43 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I61" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="N61" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O61" t="s" s="2">
         <v>40</v>
       </c>
@@ -7680,25 +7720,25 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>40</v>
@@ -7709,7 +7749,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -7732,15 +7772,17 @@
         <v>51</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="M62" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>183</v>
+      </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>40</v>
@@ -7765,13 +7807,13 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>40</v>
@@ -7789,7 +7831,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -7798,10 +7840,10 @@
         <v>50</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>40</v>
@@ -7818,7 +7860,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -7838,18 +7880,20 @@
         <v>40</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M63" s="2"/>
+        <v>189</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>40</v>
@@ -7898,7 +7942,7 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -7910,13 +7954,13 @@
         <v>40</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
@@ -7927,18 +7971,18 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>40</v>
@@ -7947,20 +7991,18 @@
         <v>40</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>40</v>
@@ -8009,25 +8051,25 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>40</v>
@@ -8038,43 +8080,39 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8122,25 +8160,25 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -8151,18 +8189,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>40</v>
@@ -8171,18 +8209,20 @@
         <v>40</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>186</v>
+        <v>121</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M66" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>40</v>
@@ -8207,13 +8247,13 @@
         <v>40</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>189</v>
+        <v>40</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>40</v>
@@ -8231,25 +8271,25 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
@@ -8260,41 +8300,43 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H67" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I67" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>191</v>
+        <v>128</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N67" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="N67" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O67" t="s" s="2">
         <v>40</v>
       </c>
@@ -8342,25 +8384,25 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>40</v>
@@ -8371,7 +8413,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8379,7 +8421,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F68" t="s" s="2">
         <v>50</v>
@@ -8394,13 +8436,13 @@
         <v>51</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8427,13 +8469,13 @@
         <v>40</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>40</v>
@@ -8451,10 +8493,10 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>50</v>
@@ -8480,7 +8522,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8488,7 +8530,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F69" t="s" s="2">
         <v>50</v>
@@ -8503,15 +8545,17 @@
         <v>51</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M69" s="2"/>
+        <v>205</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>206</v>
+      </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>40</v>
@@ -8560,10 +8604,10 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>50</v>
@@ -8589,7 +8633,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8615,10 +8659,10 @@
         <v>133</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -8669,7 +8713,7 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -8698,7 +8742,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -8721,13 +8765,13 @@
         <v>51</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -8778,7 +8822,7 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -8807,7 +8851,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -8830,13 +8874,13 @@
         <v>51</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -8887,7 +8931,7 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -8896,10 +8940,10 @@
         <v>50</v>
       </c>
       <c r="AH72" t="s" s="2">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="AJ72" t="s" s="2">
         <v>40</v>
@@ -8916,7 +8960,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -8936,16 +8980,16 @@
         <v>40</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -8996,7 +9040,7 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>116</v>
+        <v>215</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9008,13 +9052,13 @@
         <v>40</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>40</v>
@@ -9025,18 +9069,18 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>40</v>
@@ -9045,20 +9089,18 @@
         <v>40</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>123</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
         <v>40</v>
@@ -9107,25 +9149,25 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>124</v>
+        <v>218</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH74" t="s" s="2">
-        <v>40</v>
+        <v>221</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
@@ -9136,43 +9178,39 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I75" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>40</v>
       </c>
@@ -9220,25 +9258,25 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -9249,18 +9287,18 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G76" t="s" s="2">
         <v>40</v>
@@ -9269,18 +9307,20 @@
         <v>40</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="M76" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>123</v>
+      </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>40</v>
@@ -9329,25 +9369,25 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>212</v>
+        <v>124</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG76" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
@@ -9358,39 +9398,43 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H77" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I77" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="M77" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="N77" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O77" t="s" s="2">
         <v>40</v>
       </c>
@@ -9438,25 +9482,25 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>215</v>
+        <v>131</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
@@ -9467,7 +9511,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9475,7 +9519,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F78" t="s" s="2">
         <v>50</v>
@@ -9493,14 +9537,12 @@
         <v>133</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>221</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="M78" s="2"/>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
         <v>40</v>
@@ -9549,10 +9591,10 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>50</v>
@@ -9578,7 +9620,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9601,17 +9643,15 @@
         <v>51</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>40</v>
@@ -9660,7 +9700,7 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -9689,7 +9729,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -9712,16 +9752,16 @@
         <v>51</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -9771,7 +9811,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -9783,7 +9823,7 @@
         <v>40</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ80" t="s" s="2">
         <v>40</v>
@@ -9800,7 +9840,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -9823,20 +9863,18 @@
         <v>51</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>233</v>
+        <v>95</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>237</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="N81" s="2"/>
       <c r="O81" t="s" s="2">
         <v>40</v>
       </c>
@@ -9884,7 +9922,7 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -9911,8 +9949,232 @@
         <v>40</v>
       </c>
     </row>
+    <row r="82" hidden="true">
+      <c r="A82" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F82" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I82" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J82" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="K82" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="L82" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="M82" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="N82" s="2"/>
+      <c r="O82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P82" s="2"/>
+      <c r="Q82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE82" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AF82" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG82" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL82" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM82" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" hidden="true">
+      <c r="A83" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F83" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I83" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J83" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="K83" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L83" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="M83" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="O83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P83" s="2"/>
+      <c r="Q83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE83" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM83" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AM81">
+  <autoFilter ref="A1:AM83">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9922,7 +10184,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI80">
+  <conditionalFormatting sqref="A2:AI82">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>